<commit_message>
KYC and LAND Dn with form
</commit_message>
<xml_diff>
--- a/clientdata/Goat FPO QR_18112017.xlsx
+++ b/clientdata/Goat FPO QR_18112017.xlsx
@@ -1666,7 +1666,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1676,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106:C107"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3798,24 +3798,24 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="18">
+    <mergeCell ref="A5:A121"/>
+    <mergeCell ref="A261:A274"/>
+    <mergeCell ref="A275:A280"/>
+    <mergeCell ref="A281:A285"/>
+    <mergeCell ref="A122:A140"/>
+    <mergeCell ref="A141:A260"/>
+    <mergeCell ref="B59:B98"/>
+    <mergeCell ref="B99:B111"/>
+    <mergeCell ref="B122:B131"/>
+    <mergeCell ref="B132:B140"/>
+    <mergeCell ref="B5:B26"/>
+    <mergeCell ref="B27:B58"/>
     <mergeCell ref="B261:B269"/>
     <mergeCell ref="B270:B274"/>
     <mergeCell ref="B112:B121"/>
     <mergeCell ref="B141:B182"/>
     <mergeCell ref="B183:B237"/>
     <mergeCell ref="B238:B260"/>
-    <mergeCell ref="B59:B98"/>
-    <mergeCell ref="B99:B111"/>
-    <mergeCell ref="B122:B131"/>
-    <mergeCell ref="B132:B140"/>
-    <mergeCell ref="B5:B26"/>
-    <mergeCell ref="B27:B58"/>
-    <mergeCell ref="A5:A121"/>
-    <mergeCell ref="A261:A274"/>
-    <mergeCell ref="A275:A280"/>
-    <mergeCell ref="A281:A285"/>
-    <mergeCell ref="A122:A140"/>
-    <mergeCell ref="A141:A260"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Form Design dn, except goat income and expenditure and Total income bcoz of some doubts
</commit_message>
<xml_diff>
--- a/clientdata/Goat FPO QR_18112017.xlsx
+++ b/clientdata/Goat FPO QR_18112017.xlsx
@@ -1676,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C140" sqref="C140"/>
+    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C273" sqref="C273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add reg user page
</commit_message>
<xml_diff>
--- a/clientdata/Goat FPO QR_18112017.xlsx
+++ b/clientdata/Goat FPO QR_18112017.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="304">
   <si>
     <t>Survey Collector Name</t>
   </si>
@@ -974,6 +974,15 @@
   </si>
   <si>
     <t>Fields</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -1666,7 +1675,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1676,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C140" sqref="C140"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="D259" sqref="D259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3529,6 +3538,9 @@
       <c r="C252" s="20" t="s">
         <v>158</v>
       </c>
+      <c r="D252" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="46"/>
@@ -3550,6 +3562,9 @@
       <c r="C255" s="20" t="s">
         <v>161</v>
       </c>
+      <c r="D255" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="46"/>
@@ -3578,6 +3593,9 @@
       <c r="C259" s="20" t="s">
         <v>165</v>
       </c>
+      <c r="D259" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="47"/>
@@ -3798,24 +3816,24 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="18">
+    <mergeCell ref="B261:B269"/>
+    <mergeCell ref="B270:B274"/>
+    <mergeCell ref="B112:B121"/>
+    <mergeCell ref="B141:B182"/>
+    <mergeCell ref="B183:B237"/>
+    <mergeCell ref="B238:B260"/>
+    <mergeCell ref="B59:B98"/>
+    <mergeCell ref="B99:B111"/>
+    <mergeCell ref="B122:B131"/>
+    <mergeCell ref="B132:B140"/>
+    <mergeCell ref="B5:B26"/>
+    <mergeCell ref="B27:B58"/>
     <mergeCell ref="A5:A121"/>
     <mergeCell ref="A261:A274"/>
     <mergeCell ref="A275:A280"/>
     <mergeCell ref="A281:A285"/>
     <mergeCell ref="A122:A140"/>
     <mergeCell ref="A141:A260"/>
-    <mergeCell ref="B59:B98"/>
-    <mergeCell ref="B99:B111"/>
-    <mergeCell ref="B122:B131"/>
-    <mergeCell ref="B132:B140"/>
-    <mergeCell ref="B5:B26"/>
-    <mergeCell ref="B27:B58"/>
-    <mergeCell ref="B261:B269"/>
-    <mergeCell ref="B270:B274"/>
-    <mergeCell ref="B112:B121"/>
-    <mergeCell ref="B141:B182"/>
-    <mergeCell ref="B183:B237"/>
-    <mergeCell ref="B238:B260"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>